<commit_message>
Updated BOM to reflect actual weights. Switch to Aeronaut 12X10 Prop as baseline.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - BOM.xlsx
+++ b/Design/CAD/mAEWing1 - BOM.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="539">
   <si>
     <t>Description</t>
   </si>
@@ -1359,12 +1359,6 @@
     <t>Aeronaut </t>
   </si>
   <si>
-    <t>Yoke 38/8</t>
-  </si>
-  <si>
-    <t>Yoke for folding prop, 38mm pin-to-pin</t>
-  </si>
-  <si>
     <t>http://www.espritmodel.com/aeronaut-yoke-for-turbo-and-black-spinners.aspx</t>
   </si>
   <si>
@@ -1633,6 +1627,27 @@
   </si>
   <si>
     <t>http://hobbyking.com/hobbyking/store/__32011__HobbyKing_Glider_Nose_Tow_Line_Release_11_7x42mm_US_Warehouse_.html</t>
+  </si>
+  <si>
+    <t>With shortened coax cable, removed cover</t>
+  </si>
+  <si>
+    <t>AER7234/49</t>
+  </si>
+  <si>
+    <t>http://www.espritmodel.com/aeronaut-cam-folding-propellers-rudi-freudenthaler.aspx</t>
+  </si>
+  <si>
+    <t>AER724221</t>
+  </si>
+  <si>
+    <t>Yoke for folding prop, 38mm pin-to-pin, 8mm shoulder</t>
+  </si>
+  <si>
+    <t>Folding 12" X 10"</t>
+  </si>
+  <si>
+    <t>Alternate Prop - Folding 12" X 10"</t>
   </si>
 </sst>
 </file>
@@ -2194,7 +2209,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2292,7 +2307,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B14" t="s">
         <v>228</v>
@@ -2306,7 +2321,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>228</v>
@@ -2315,7 +2330,7 @@
         <v>42125</v>
       </c>
       <c r="D15" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2630,19 +2645,19 @@
         <v/>
       </c>
       <c r="M4" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="O4" s="2">
         <v>24</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3727,7 +3742,7 @@
         <v/>
       </c>
       <c r="M24" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2">
@@ -3783,14 +3798,14 @@
         <v/>
       </c>
       <c r="M25" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2">
         <v>1</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Q25" s="2"/>
     </row>
@@ -3833,7 +3848,7 @@
         <v/>
       </c>
       <c r="M26" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2">
@@ -4537,16 +4552,16 @@
         <v/>
       </c>
       <c r="M39" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="O39" s="2">
         <v>1</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="Q39" s="2"/>
     </row>
@@ -4589,7 +4604,7 @@
         <v/>
       </c>
       <c r="M40" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2">
@@ -4641,7 +4656,7 @@
         <v/>
       </c>
       <c r="M41" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2">
@@ -6883,17 +6898,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B81:Q81"/>
-    <mergeCell ref="B82:Q82"/>
-    <mergeCell ref="B83:Q83"/>
-    <mergeCell ref="B84:Q84"/>
-    <mergeCell ref="B85:Q85"/>
     <mergeCell ref="B91:Q91"/>
     <mergeCell ref="B86:Q86"/>
     <mergeCell ref="B87:Q87"/>
     <mergeCell ref="B88:Q88"/>
     <mergeCell ref="B89:Q89"/>
     <mergeCell ref="B90:Q90"/>
+    <mergeCell ref="B81:Q81"/>
+    <mergeCell ref="B82:Q82"/>
+    <mergeCell ref="B83:Q83"/>
+    <mergeCell ref="B84:Q84"/>
+    <mergeCell ref="B85:Q85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6902,11 +6917,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V102"/>
+  <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="A51:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7393,7 +7408,9 @@
       <c r="G11" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>532</v>
+      </c>
       <c r="J11" s="3">
         <v>50</v>
       </c>
@@ -7405,20 +7422,20 @@
         <v>197</v>
       </c>
       <c r="M11" s="2">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="N11" s="2">
         <f>F11*M11</f>
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>198</v>
       </c>
       <c r="R11" s="29" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -7455,14 +7472,14 @@
         <v>194</v>
       </c>
       <c r="M13" s="2">
-        <v>9.4</v>
+        <v>10</v>
       </c>
       <c r="N13" s="2">
         <f>F13*M13</f>
-        <v>9.4</v>
+        <v>10</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>211</v>
@@ -7505,14 +7522,14 @@
         <v>194</v>
       </c>
       <c r="M14" s="4">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="N14" s="4">
         <f>F14*M14</f>
-        <v>139</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>195</v>
+        <v>132</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>430</v>
@@ -7529,13 +7546,13 @@
         <v>377</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="E15" s="47" t="s">
         <v>489</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>491</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -7555,18 +7572,18 @@
         <v>194</v>
       </c>
       <c r="M15" s="4">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="N15" s="4">
         <f>F15*M15</f>
-        <v>58</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>195</v>
+        <v>68</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="P15" s="4"/>
       <c r="R15" s="49" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -7690,7 +7707,7 @@
         <v>360</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J19" s="3">
         <v>15</v>
@@ -7714,7 +7731,7 @@
       </c>
       <c r="P19" s="2"/>
       <c r="R19" s="29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -7741,7 +7758,7 @@
         <v>360</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J20" s="3">
         <v>3.75</v>
@@ -7765,7 +7782,7 @@
       </c>
       <c r="P20" s="2"/>
       <c r="R20" s="29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -7869,7 +7886,7 @@
       </c>
       <c r="P22" s="2"/>
       <c r="R22" s="51" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -8045,7 +8062,7 @@
         <v>360</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J27" s="3">
         <v>15</v>
@@ -8069,7 +8086,7 @@
       </c>
       <c r="P27" s="2"/>
       <c r="R27" s="29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -8096,7 +8113,7 @@
         <v>360</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J28" s="3">
         <v>3.75</v>
@@ -8120,7 +8137,7 @@
       </c>
       <c r="P28" s="2"/>
       <c r="R28" s="29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -8224,7 +8241,7 @@
       </c>
       <c r="P30" s="2"/>
       <c r="R30" s="51" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -8306,7 +8323,7 @@
         <v>109.99</v>
       </c>
       <c r="K33" s="3">
-        <f t="shared" ref="K33:K38" si="6">F33*J33</f>
+        <f t="shared" ref="K33:K39" si="6">F33*J33</f>
         <v>109.99</v>
       </c>
       <c r="L33" s="3" t="s">
@@ -8316,7 +8333,7 @@
         <v>357</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" ref="N33:N38" si="7">F33*M33</f>
+        <f t="shared" ref="N33:N39" si="7">F33*M33</f>
         <v>357</v>
       </c>
       <c r="O33" s="2" t="s">
@@ -8324,7 +8341,7 @@
       </c>
       <c r="P33" s="2"/>
       <c r="R33" s="29" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -8372,7 +8389,7 @@
       </c>
       <c r="P34" s="2"/>
       <c r="R34" s="29" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -8442,31 +8459,33 @@
         <v>99</v>
       </c>
       <c r="F36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>538</v>
+      </c>
       <c r="J36" s="3">
         <v>35</v>
       </c>
       <c r="K36" s="3">
         <f t="shared" si="6"/>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>194</v>
       </c>
       <c r="M36" s="2">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="N36" s="2">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P36" s="2"/>
       <c r="R36" s="29" t="s">
@@ -8481,13 +8500,13 @@
         <v>368</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>435</v>
+        <v>94</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>441</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>442</v>
+        <v>533</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -8496,31 +8515,31 @@
         <v>360</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>443</v>
+        <v>537</v>
       </c>
       <c r="J37" s="3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="6"/>
-        <v>9</v>
+        <f t="shared" ref="K37" si="8">F37*J37</f>
+        <v>13</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>194</v>
       </c>
       <c r="M37" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" ref="N37" si="9">F37*M37</f>
+        <v>16</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P37" s="2"/>
       <c r="R37" s="29" t="s">
-        <v>444</v>
+        <v>534</v>
       </c>
     </row>
     <row r="38" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8531,13 +8550,13 @@
         <v>368</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>438</v>
+        <v>535</v>
       </c>
       <c r="F38" s="2">
         <v>1</v>
@@ -8546,102 +8565,100 @@
         <v>360</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>439</v>
+        <v>536</v>
       </c>
       <c r="J38" s="3">
-        <v>5.49</v>
+        <v>9</v>
       </c>
       <c r="K38" s="3">
         <f t="shared" si="6"/>
-        <v>5.49</v>
+        <v>9</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>194</v>
       </c>
       <c r="M38" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N38" s="2">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P38" s="2"/>
       <c r="R38" s="29" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="R39" s="35"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A39" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F41" s="2">
-        <v>6</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="J41" s="3">
-        <f>12.09+8.54</f>
-        <v>20.63</v>
-      </c>
-      <c r="K41" s="3">
-        <f>F41*J41</f>
-        <v>123.78</v>
-      </c>
-      <c r="L41" s="3" t="s">
+      <c r="H39" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="J39" s="3">
+        <v>5.49</v>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" si="6"/>
+        <v>5.49</v>
+      </c>
+      <c r="L39" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="M41" s="33">
-        <f>17/6</f>
-        <v>2.8333333333333335</v>
-      </c>
-      <c r="N41" s="2">
-        <f>F41*M41</f>
-        <v>17</v>
-      </c>
-      <c r="O41" s="2" t="s">
+      <c r="M39" s="2">
+        <v>23</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="O39" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="P41" s="2"/>
-      <c r="R41" s="29" t="s">
-        <v>463</v>
-      </c>
+      <c r="P39" s="2"/>
+      <c r="R39" s="29" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="R40" s="35"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -8651,45 +8668,49 @@
         <v>367</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="F42" s="2">
+        <v>6</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J42" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K42" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="L42" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M42" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="N42" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="O42" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="P42" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="R42" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="J42" s="3">
+        <f>12.09+8.54</f>
+        <v>20.63</v>
+      </c>
+      <c r="K42" s="3">
+        <f>F42*J42</f>
+        <v>123.78</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M42" s="33">
+        <f>17/6</f>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="N42" s="2">
+        <f>F42*M42</f>
+        <v>17</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="P42" s="2"/>
+      <c r="R42" s="29" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -8699,48 +8720,45 @@
         <v>367</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F43" s="2">
-        <v>2</v>
+        <v>151</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="J43" s="3">
-        <f>12.79+8.94</f>
-        <v>21.729999999999997</v>
-      </c>
-      <c r="K43" s="3">
-        <f>F43*J43</f>
-        <v>43.459999999999994</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="M43" s="2">
-        <v>8</v>
-      </c>
-      <c r="N43" s="2">
-        <f>F43*M43</f>
-        <v>16</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="P43" s="2"/>
-      <c r="R43" s="29" t="s">
-        <v>464</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L43" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M43" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N43" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O43" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="P43" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R43" s="2"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -8750,45 +8768,48 @@
         <v>367</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>152</v>
+        <v>241</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H44" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="J44" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K44" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="L44" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M44" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="N44" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="O44" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="P44" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="R44" s="21"/>
+      <c r="H44" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="J44" s="3">
+        <f>12.79+8.94</f>
+        <v>21.729999999999997</v>
+      </c>
+      <c r="K44" s="3">
+        <f>F44*J44</f>
+        <v>43.459999999999994</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M44" s="2">
+        <v>8</v>
+      </c>
+      <c r="N44" s="2">
+        <f>F44*M44</f>
+        <v>16</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="P44" s="2"/>
+      <c r="R44" s="29" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -8798,31 +8819,31 @@
         <v>367</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="E45" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F45" s="2">
-        <f>F41</f>
-        <v>6</v>
+        <v>147</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="J45" s="3">
-        <v>0.37</v>
-      </c>
-      <c r="K45" s="3">
-        <f>F45*J45</f>
-        <v>2.2199999999999998</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>194</v>
+      <c r="H45" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="M45" s="18" t="s">
         <v>2</v>
@@ -8836,9 +8857,7 @@
       <c r="P45" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R45" s="29" t="s">
-        <v>404</v>
-      </c>
+      <c r="R45" s="21"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -8848,28 +8867,28 @@
         <v>367</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F46" s="2">
-        <f>F41</f>
+        <f>F42</f>
         <v>6</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>141</v>
+        <v>258</v>
       </c>
       <c r="J46" s="3">
-        <v>0.59</v>
+        <v>0.37</v>
       </c>
       <c r="K46" s="3">
         <f>F46*J46</f>
-        <v>3.54</v>
+        <v>2.2199999999999998</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>194</v>
@@ -8887,7 +8906,7 @@
         <v>2</v>
       </c>
       <c r="R46" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -8898,28 +8917,28 @@
         <v>367</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F47" s="2">
-        <f>F43</f>
-        <v>2</v>
+        <f>F42</f>
+        <v>6</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J47" s="3">
-        <v>0.38</v>
+        <v>0.59</v>
       </c>
       <c r="K47" s="3">
         <f>F47*J47</f>
-        <v>0.76</v>
+        <v>3.54</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>194</v>
@@ -8937,62 +8956,60 @@
         <v>2</v>
       </c>
       <c r="R47" s="29" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F48" s="2">
+        <f>F44</f>
+        <v>2</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="K48" s="3">
+        <f>F48*J48</f>
+        <v>0.76</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M48" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N48" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O48" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="P48" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R48" s="29" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F49" s="2">
-        <v>1</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="J49" s="3">
-        <v>8.49</v>
-      </c>
-      <c r="K49" s="3">
-        <f>J49*F49</f>
-        <v>8.49</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="M49" s="2">
-        <v>3</v>
-      </c>
-      <c r="N49" s="2">
-        <f>F49*M49</f>
-        <v>3</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="R49" s="29" t="s">
-        <v>461</v>
-      </c>
-    </row>
+    <row r="49" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>388</v>
@@ -9001,41 +9018,49 @@
         <v>391</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="F50" s="2">
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H50" s="50" t="s">
-        <v>462</v>
+      <c r="H50" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="J50" s="3">
-        <v>5</v>
+        <v>8.49</v>
       </c>
       <c r="K50" s="3">
         <f>J50*F50</f>
-        <v>5</v>
+        <v>8.49</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M50" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="N50" s="2">
         <f>F50*M50</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="P50" s="2"/>
-      <c r="R50" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="R50" s="29" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -9045,49 +9070,43 @@
         <v>391</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>448</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="12"/>
       <c r="F51" s="2">
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>511</v>
+      <c r="H51" s="50" t="s">
+        <v>460</v>
       </c>
       <c r="J51" s="3">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="K51" s="3">
         <f>J51*F51</f>
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>197</v>
       </c>
       <c r="M51" s="2">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="N51" s="2">
         <f>F51*M51</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>196</v>
       </c>
       <c r="P51" s="2"/>
-      <c r="R51" s="29" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>388</v>
       </c>
@@ -9095,13 +9114,13 @@
         <v>391</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>67</v>
+        <v>447</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -9110,7 +9129,7 @@
         <v>360</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="J52" s="3">
         <v>40</v>
@@ -9134,61 +9153,61 @@
       </c>
       <c r="P52" s="2"/>
       <c r="R52" s="29" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="F54" s="4">
+      <c r="B53" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="F53" s="2">
         <v>1</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H54" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="J54" s="10">
-        <v>122.95</v>
-      </c>
-      <c r="K54" s="3">
-        <f t="shared" ref="K54:K57" si="8">J54*F54</f>
-        <v>122.95</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M54" s="2">
-        <v>38</v>
-      </c>
-      <c r="N54" s="2">
-        <f>F54*M54</f>
-        <v>38</v>
-      </c>
-      <c r="O54" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="R54" s="49" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="J53" s="3">
+        <v>40</v>
+      </c>
+      <c r="K53" s="3">
+        <f>J53*F53</f>
+        <v>40</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="M53" s="2">
+        <v>3</v>
+      </c>
+      <c r="N53" s="2">
+        <f>F53*M53</f>
+        <v>3</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="R53" s="29" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>388</v>
       </c>
@@ -9196,13 +9215,13 @@
         <v>366</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>451</v>
+        <v>45</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>300</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>456</v>
+        <v>301</v>
       </c>
       <c r="F55" s="4">
         <v>1</v>
@@ -9211,31 +9230,31 @@
         <v>360</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="J55" s="10">
-        <v>14.95</v>
+        <v>122.95</v>
       </c>
       <c r="K55" s="3">
-        <f t="shared" si="8"/>
-        <v>14.95</v>
+        <f t="shared" ref="K55:K58" si="10">J55*F55</f>
+        <v>122.95</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M55" s="2">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="N55" s="2">
-        <f t="shared" ref="N55:N56" si="9">F55*M55</f>
-        <v>5</v>
+        <f>F55*M55</f>
+        <v>38</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P55" s="2"/>
       <c r="R55" s="49" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="56" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9246,11 +9265,13 @@
         <v>366</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="D56" s="4"/>
+        <v>449</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>300</v>
+      </c>
       <c r="E56" s="4" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F56" s="4">
         <v>1</v>
@@ -9258,31 +9279,35 @@
       <c r="G56" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H56" s="4"/>
+      <c r="H56" s="4" t="s">
+        <v>455</v>
+      </c>
       <c r="J56" s="10">
-        <v>5</v>
+        <v>14.95</v>
       </c>
       <c r="K56" s="3">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <f t="shared" si="10"/>
+        <v>14.95</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M56" s="2">
         <v>5</v>
       </c>
       <c r="N56" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="N56:N57" si="11">F56*M56</f>
         <v>5</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>196</v>
       </c>
       <c r="P56" s="2"/>
-      <c r="R56" s="4"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R56" s="49" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>388</v>
       </c>
@@ -9290,13 +9315,11 @@
         <v>366</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>249</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="F57" s="4">
         <v>1</v>
@@ -9304,96 +9327,92 @@
       <c r="G57" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="H57" s="4"/>
+      <c r="J57" s="10">
+        <v>5</v>
+      </c>
+      <c r="K57" s="3">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M57" s="2">
+        <v>5</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="R57" s="4"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="F58" s="4">
+        <v>1</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="J57" s="10">
+      <c r="J58" s="10">
         <v>64.989999999999995</v>
       </c>
-      <c r="K57" s="3">
-        <f t="shared" si="8"/>
+      <c r="K58" s="3">
+        <f t="shared" si="10"/>
         <v>64.989999999999995</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="L58" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="M57" s="2">
+      <c r="M58" s="2">
         <v>23</v>
       </c>
-      <c r="N57" s="2">
-        <f>F57*M57</f>
+      <c r="N58" s="2">
+        <f>F58*M58</f>
         <v>23</v>
       </c>
-      <c r="O57" s="2" t="s">
+      <c r="O58" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="P57" s="2"/>
-      <c r="R57" s="49" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-    </row>
-    <row r="59" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P58" s="2"/>
+      <c r="R58" s="49" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C59" s="15"/>
       <c r="D59" s="15"/>
-      <c r="E59" s="40"/>
+      <c r="E59" s="31"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F60" s="2">
-        <v>4</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J60" s="3">
-        <f>1.04/4</f>
-        <v>0.26</v>
-      </c>
-      <c r="K60" s="3">
-        <f>F60*J60</f>
-        <v>1.04</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M60" s="2">
-        <v>0</v>
-      </c>
-      <c r="N60" s="2">
-        <f t="shared" ref="N60:N99" si="10">F60*M60</f>
-        <v>0</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="16"/>
-      <c r="R60" s="29" t="s">
-        <v>343</v>
-      </c>
+    <row r="60" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="15"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
@@ -9403,11 +9422,11 @@
         <v>382</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>265</v>
+        <v>477</v>
       </c>
       <c r="F61" s="2">
         <v>4</v>
@@ -9416,15 +9435,15 @@
         <v>360</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
       <c r="J61" s="3">
-        <f>6.63/50</f>
-        <v>0.1326</v>
+        <f>1.04/4</f>
+        <v>0.26</v>
       </c>
       <c r="K61" s="3">
         <f>F61*J61</f>
-        <v>0.53039999999999998</v>
+        <v>1.04</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>194</v>
@@ -9433,7 +9452,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="N61:N100" si="12">F61*M61</f>
         <v>0</v>
       </c>
       <c r="O61" s="2" t="s">
@@ -9442,59 +9461,62 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="16"/>
       <c r="R61" s="29" t="s">
-        <v>483</v>
+        <v>343</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q62" s="37"/>
-      <c r="R62"/>
+      <c r="A62" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F62" s="2">
+        <v>4</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J62" s="3">
+        <f>6.63/50</f>
+        <v>0.1326</v>
+      </c>
+      <c r="K62" s="3">
+        <f>F62*J62</f>
+        <v>0.53039999999999998</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M62" s="2">
+        <v>0</v>
+      </c>
+      <c r="N62" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="29" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="F63" s="2">
-        <v>12</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H63" s="2"/>
-      <c r="J63" s="3">
-        <v>0.21</v>
-      </c>
-      <c r="K63" s="3">
-        <f>F63*J63</f>
-        <v>2.52</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M63" s="2">
-        <v>3</v>
-      </c>
-      <c r="N63" s="2">
-        <f t="shared" si="10"/>
-        <v>36</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="16"/>
-      <c r="R63" s="29" t="s">
-        <v>531</v>
-      </c>
+      <c r="Q63" s="37"/>
+      <c r="R63"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -9504,14 +9526,13 @@
         <v>381</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F64" s="2">
-        <f>F63</f>
         <v>12</v>
       </c>
       <c r="G64" s="2" t="s">
@@ -9519,21 +9540,21 @@
       </c>
       <c r="H64" s="2"/>
       <c r="J64" s="3">
-        <v>0.06</v>
+        <v>0.21</v>
       </c>
       <c r="K64" s="3">
         <f>F64*J64</f>
-        <v>0.72</v>
+        <v>2.52</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M64" s="2">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="N64" s="2">
-        <f t="shared" si="10"/>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>36</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>196</v>
@@ -9541,73 +9562,71 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="16"/>
       <c r="R64" s="29" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65"/>
-      <c r="M65"/>
-      <c r="N65"/>
-      <c r="O65"/>
-      <c r="P65"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F65" s="2">
+        <f>F64</f>
+        <v>12</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H65" s="2"/>
+      <c r="J65" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="K65" s="3">
+        <f>F65*J65</f>
+        <v>0.72</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M65" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="N65" s="2">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P65" s="2"/>
       <c r="Q65" s="16"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F66" s="2">
-        <v>2</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="J66" s="3">
-        <f>32/100</f>
-        <v>0.32</v>
-      </c>
-      <c r="K66" s="3">
-        <f>F66*J66</f>
-        <v>0.64</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M66" s="2">
-        <v>5</v>
-      </c>
-      <c r="N66" s="2">
-        <f t="shared" si="10"/>
-        <v>10</v>
-      </c>
-      <c r="O66" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="P66" s="2"/>
+      <c r="R65" s="29" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
       <c r="Q66" s="16"/>
-      <c r="R66" s="29" t="s">
-        <v>529</v>
-      </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
@@ -9617,36 +9636,38 @@
         <v>383</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
-        <v>395</v>
+        <v>263</v>
       </c>
       <c r="F67" s="2">
-        <f>F66</f>
         <v>2</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H67" s="2"/>
+      <c r="H67" s="2" t="s">
+        <v>396</v>
+      </c>
       <c r="J67" s="3">
-        <v>0.12</v>
+        <f>32/100</f>
+        <v>0.32</v>
       </c>
       <c r="K67" s="3">
         <f>F67*J67</f>
-        <v>0.24</v>
+        <v>0.64</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M67" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N67" s="2">
-        <f t="shared" si="10"/>
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>10</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>196</v>
@@ -9654,76 +9675,76 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="16"/>
       <c r="R67" s="29" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="G68"/>
-      <c r="R68"/>
-    </row>
-    <row r="69" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A68" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F69" s="2">
+      <c r="B68" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F68" s="2">
+        <f>F67</f>
         <v>2</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H69" s="2"/>
-      <c r="J69" s="3">
-        <f>32/100</f>
-        <v>0.32</v>
-      </c>
-      <c r="K69" s="3">
-        <f>F69*J69</f>
-        <v>0.64</v>
-      </c>
-      <c r="L69" s="2" t="s">
+      <c r="H68" s="2"/>
+      <c r="J68" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K68" s="3">
+        <f>F68*J68</f>
+        <v>0.24</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="M69" s="2">
-        <v>5</v>
-      </c>
-      <c r="N69" s="2">
-        <f>F69*M69</f>
-        <v>10</v>
-      </c>
-      <c r="O69" s="2" t="s">
+      <c r="M68" s="2">
+        <v>3</v>
+      </c>
+      <c r="N68" s="2">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="O68" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="P69" s="2"/>
-      <c r="Q69" s="16"/>
-      <c r="R69" s="29" t="s">
-        <v>529</v>
-      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="29" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="G69"/>
+      <c r="R69"/>
     </row>
     <row r="70" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>389</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>481</v>
+        <v>263</v>
       </c>
       <c r="F70" s="2">
         <v>2</v>
@@ -9733,22 +9754,22 @@
       </c>
       <c r="H70" s="2"/>
       <c r="J70" s="3">
-        <f>1.36/4</f>
-        <v>0.34</v>
+        <f>32/100</f>
+        <v>0.32</v>
       </c>
       <c r="K70" s="3">
         <f>F70*J70</f>
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M70" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N70" s="2">
         <f>F70*M70</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O70" s="2" t="s">
         <v>196</v>
@@ -9756,107 +9777,106 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="16"/>
       <c r="R70" s="29" t="s">
-        <v>482</v>
+        <v>527</v>
       </c>
     </row>
     <row r="71" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="2"/>
+      <c r="A71" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="F71" s="2">
+        <v>2</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="H71" s="2"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
+      <c r="J71" s="3">
+        <f>1.36/4</f>
+        <v>0.34</v>
+      </c>
+      <c r="K71" s="3">
+        <f>F71*J71</f>
+        <v>0.68</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M71" s="2">
+        <v>2</v>
+      </c>
+      <c r="N71" s="2">
+        <f>F71*M71</f>
+        <v>4</v>
+      </c>
+      <c r="O71" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="P71" s="2"/>
       <c r="Q71" s="16"/>
-      <c r="R71" s="29"/>
+      <c r="R71" s="29" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="72" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>517</v>
-      </c>
+      <c r="A72" s="2"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F72" s="2">
-        <v>8</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="J72" s="3">
-        <f>1.04/4</f>
-        <v>0.26</v>
-      </c>
-      <c r="K72" s="3">
-        <f>F72*J72</f>
-        <v>2.08</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M72" s="2">
-        <v>0</v>
-      </c>
-      <c r="N72" s="2">
-        <f t="shared" ref="N72:N75" si="11">F72*M72</f>
-        <v>0</v>
-      </c>
-      <c r="O72" s="2" t="s">
-        <v>196</v>
-      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
       <c r="P72" s="2"/>
       <c r="Q72" s="16"/>
-      <c r="R72" s="29" t="s">
-        <v>343</v>
-      </c>
+      <c r="R72" s="29"/>
     </row>
     <row r="73" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>389</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2" t="s">
-        <v>526</v>
+        <v>477</v>
       </c>
       <c r="F73" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="J73" s="3">
-        <v>0.05</v>
+        <f>1.04/4</f>
+        <v>0.26</v>
       </c>
       <c r="K73" s="3">
         <f>F73*J73</f>
-        <v>0.2</v>
+        <v>2.08</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>194</v>
@@ -9865,7 +9885,7 @@
         <v>0</v>
       </c>
       <c r="N73" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="N73:N76" si="13">F73*M73</f>
         <v>0</v>
       </c>
       <c r="O73" s="2" t="s">
@@ -9874,7 +9894,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="16"/>
       <c r="R73" s="29" t="s">
-        <v>527</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9882,14 +9902,14 @@
         <v>389</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="F74" s="2">
         <v>4</v>
@@ -9898,21 +9918,23 @@
         <v>360</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="J74" s="3">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="K74" s="3">
-        <f t="shared" ref="K74:K75" si="12">F74*J74</f>
-        <v>0.24</v>
+        <f>F74*J74</f>
+        <v>0.2</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="M74" s="2"/>
+      <c r="M74" s="2">
+        <v>0</v>
+      </c>
       <c r="N74" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O74" s="2" t="s">
@@ -9921,7 +9943,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="16"/>
       <c r="R74" s="29" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="75" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9929,33 +9951,37 @@
         <v>389</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>517</v>
+      </c>
       <c r="F75" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H75" s="2"/>
+      <c r="H75" s="2" t="s">
+        <v>519</v>
+      </c>
       <c r="J75" s="3">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="K75" s="3">
-        <f t="shared" si="12"/>
-        <v>0.1</v>
+        <f t="shared" ref="K75:K76" si="14">F75*J75</f>
+        <v>0.24</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O75" s="2" t="s">
@@ -9963,142 +9989,136 @@
       </c>
       <c r="P75" s="2"/>
       <c r="Q75" s="16"/>
-      <c r="R75" s="29"/>
+      <c r="R75" s="29" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="76" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="J76" s="16"/>
-      <c r="K76" s="16"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="14"/>
-      <c r="N76" s="14"/>
-      <c r="O76" s="14"/>
-      <c r="P76" s="14"/>
+      <c r="A76" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2">
+        <v>2</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H76" s="2"/>
+      <c r="J76" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K76" s="3">
+        <f t="shared" si="14"/>
+        <v>0.1</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="P76" s="2"/>
       <c r="Q76" s="16"/>
-      <c r="R76" s="35"/>
+      <c r="R76" s="29"/>
     </row>
     <row r="77" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="14"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="16"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="16"/>
+      <c r="R77" s="35"/>
+    </row>
+    <row r="78" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2">
+      <c r="B78" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2">
         <v>2</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H77" s="2"/>
-      <c r="J77" s="3">
+      <c r="H78" s="2"/>
+      <c r="J78" s="3">
         <v>0.05</v>
       </c>
-      <c r="K77" s="3">
-        <f t="shared" ref="K77" si="13">F77*J77</f>
+      <c r="K78" s="3">
+        <f t="shared" ref="K78" si="15">F78*J78</f>
         <v>0.1</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="L78" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2">
-        <f t="shared" ref="N77" si="14">F77*M77</f>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2">
+        <f t="shared" ref="N78" si="16">F78*M78</f>
         <v>0</v>
       </c>
-      <c r="O77" s="2" t="s">
+      <c r="O78" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="16"/>
-      <c r="R77" s="29"/>
-    </row>
-    <row r="78" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="15"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
-      <c r="L78"/>
-      <c r="M78"/>
-      <c r="N78"/>
-      <c r="O78"/>
-      <c r="P78"/>
+      <c r="P78" s="2"/>
       <c r="Q78" s="16"/>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J79" s="13"/>
+      <c r="R78" s="29"/>
+    </row>
+    <row r="79" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="15"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="J79" s="16"/>
       <c r="K79" s="16"/>
+      <c r="L79"/>
+      <c r="M79"/>
+      <c r="N79"/>
+      <c r="O79"/>
+      <c r="P79"/>
       <c r="Q79" s="16"/>
-      <c r="R79" s="39" t="s">
-        <v>510</v>
-      </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="F80" s="2">
-        <v>8</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="J80" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="K80" s="3">
-        <f>J80*F80</f>
-        <v>1.6</v>
-      </c>
-      <c r="L80" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="M80" s="2">
-        <v>1</v>
-      </c>
-      <c r="N80" s="2">
-        <f>F80*M80</f>
-        <v>8</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="P80" s="2"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="16"/>
       <c r="Q80" s="16"/>
-      <c r="R80" s="29" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R80" s="39" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>390</v>
       </c>
@@ -10106,11 +10126,11 @@
         <v>392</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>514</v>
+        <v>237</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F81" s="2">
         <v>8</v>
@@ -10119,7 +10139,7 @@
         <v>360</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J81" s="3">
         <v>0.2</v>
@@ -10144,10 +10164,10 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="16"/>
       <c r="R81" s="29" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>390</v>
       </c>
@@ -10155,21 +10175,20 @@
         <v>392</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F82" s="2">
-        <f>F81</f>
         <v>8</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="J82" s="3">
         <v>0.2</v>
@@ -10194,10 +10213,10 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="16"/>
       <c r="R82" s="29" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>390</v>
       </c>
@@ -10205,36 +10224,38 @@
         <v>392</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>493</v>
+        <v>513</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="F83" s="2">
-        <f>3*F82</f>
-        <v>24</v>
+        <f>F82</f>
+        <v>8</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="H83" s="2"/>
+      <c r="H83" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="J83" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K83" s="3">
-        <f t="shared" ref="K83:K84" si="15">J83*F83</f>
-        <v>2.4000000000000004</v>
+        <f>J83*F83</f>
+        <v>1.6</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>196</v>
       </c>
       <c r="M83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N83" s="2">
         <f>F83*M83</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O83" s="2" t="s">
         <v>197</v>
@@ -10253,14 +10274,14 @@
         <v>392</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F84" s="2">
-        <f>3*F80</f>
+        <f>3*F83</f>
         <v>24</v>
       </c>
       <c r="G84" s="2" t="s">
@@ -10271,7 +10292,7 @@
         <v>0.1</v>
       </c>
       <c r="K84" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="K84:K85" si="17">J84*F84</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="L84" s="2" t="s">
@@ -10290,10 +10311,10 @@
       <c r="P84" s="2"/>
       <c r="Q84" s="16"/>
       <c r="R84" s="29" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>390</v>
       </c>
@@ -10301,40 +10322,36 @@
         <v>392</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>281</v>
-      </c>
+        <v>492</v>
+      </c>
+      <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
-        <v>282</v>
+        <v>494</v>
       </c>
       <c r="F85" s="2">
-        <v>20</v>
+        <f>3*F81</f>
+        <v>24</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>397</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="H85" s="2"/>
       <c r="J85" s="3">
-        <f>15.39/50</f>
-        <v>0.30780000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="K85" s="3">
-        <f>J85*F85</f>
-        <v>6.1560000000000006</v>
+        <f t="shared" si="17"/>
+        <v>2.4000000000000004</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M85" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N85" s="2">
-        <f t="shared" si="10"/>
-        <v>60</v>
+        <f>F85*M85</f>
+        <v>0</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>197</v>
@@ -10342,66 +10359,67 @@
       <c r="P85" s="2"/>
       <c r="Q85" s="16"/>
       <c r="R85" s="29" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F86" s="2">
+        <v>20</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J86" s="3">
+        <f>15.39/50</f>
+        <v>0.30780000000000002</v>
+      </c>
+      <c r="K86" s="3">
+        <f>J86*F86</f>
+        <v>6.1560000000000006</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M86" s="2">
+        <v>3</v>
+      </c>
+      <c r="N86" s="2">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="16"/>
+      <c r="R86" s="29" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="86" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="L86"/>
-      <c r="M86"/>
-      <c r="N86"/>
-      <c r="O86"/>
-      <c r="P86"/>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F87" s="2">
-        <v>1</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H87" s="2"/>
-      <c r="I87" s="37"/>
-      <c r="J87" s="3">
-        <f>3.19/2</f>
-        <v>1.595</v>
-      </c>
-      <c r="K87" s="3">
-        <f t="shared" ref="K87:K93" si="16">J87*F87</f>
-        <v>1.595</v>
-      </c>
-      <c r="L87" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M87" s="2">
-        <v>3</v>
-      </c>
-      <c r="N87" s="2">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="O87" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="P87" s="2"/>
-      <c r="Q87" s="16"/>
-      <c r="R87" s="29" t="s">
-        <v>341</v>
-      </c>
+    <row r="87" spans="1:22" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L87"/>
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+      <c r="P87"/>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -10411,37 +10429,39 @@
         <v>393</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>271</v>
+        <v>339</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>259</v>
+        <v>313</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
       <c r="F88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>360</v>
       </c>
       <c r="H88" s="2"/>
+      <c r="I88" s="37"/>
       <c r="J88" s="3">
-        <v>0.19</v>
+        <f>3.19/2</f>
+        <v>1.595</v>
       </c>
       <c r="K88" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" ref="K88:K94" si="18">J88*F88</f>
+        <v>1.595</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M88" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N88" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>3</v>
       </c>
       <c r="O88" s="2" t="s">
         <v>197</v>
@@ -10449,7 +10469,7 @@
       <c r="P88" s="2"/>
       <c r="Q88" s="16"/>
       <c r="R88" s="29" t="s">
-        <v>402</v>
+        <v>341</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
@@ -10466,10 +10486,9 @@
         <v>259</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F89" s="2">
-        <f>2*F88</f>
         <v>0</v>
       </c>
       <c r="G89" s="2" t="s">
@@ -10477,10 +10496,10 @@
       </c>
       <c r="H89" s="2"/>
       <c r="J89" s="3">
-        <v>0.11</v>
+        <v>0.19</v>
       </c>
       <c r="K89" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L89" s="2" t="s">
@@ -10490,7 +10509,7 @@
         <v>1</v>
       </c>
       <c r="N89" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O89" s="2" t="s">
@@ -10499,7 +10518,7 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="16"/>
       <c r="R89" s="29" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
@@ -10516,9 +10535,10 @@
         <v>259</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F90" s="2">
+        <f>2*F89</f>
         <v>0</v>
       </c>
       <c r="G90" s="2" t="s">
@@ -10526,10 +10546,10 @@
       </c>
       <c r="H90" s="2"/>
       <c r="J90" s="3">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="K90" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L90" s="2" t="s">
@@ -10539,7 +10559,7 @@
         <v>1</v>
       </c>
       <c r="N90" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O90" s="2" t="s">
@@ -10548,7 +10568,7 @@
       <c r="P90" s="2"/>
       <c r="Q90" s="16"/>
       <c r="R90" s="29" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
@@ -10565,10 +10585,9 @@
         <v>259</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F91" s="2">
-        <f>2*F90</f>
         <v>0</v>
       </c>
       <c r="G91" s="2" t="s">
@@ -10576,10 +10595,10 @@
       </c>
       <c r="H91" s="2"/>
       <c r="J91" s="3">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="K91" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L91" s="2" t="s">
@@ -10589,7 +10608,7 @@
         <v>1</v>
       </c>
       <c r="N91" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O91" s="2" t="s">
@@ -10598,7 +10617,7 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="16"/>
       <c r="R91" s="29" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
@@ -10609,37 +10628,37 @@
         <v>393</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>268</v>
+        <v>312</v>
       </c>
       <c r="F92" s="2">
+        <f>2*F91</f>
         <v>0</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H92" s="2"/>
       <c r="J92" s="3">
-        <f>23.63/25</f>
-        <v>0.94519999999999993</v>
+        <v>0.11</v>
       </c>
       <c r="K92" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M92" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N92" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O92" s="2" t="s">
@@ -10648,7 +10667,7 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="16"/>
       <c r="R92" s="29" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
@@ -10659,13 +10678,13 @@
         <v>393</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>266</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F93" s="2">
         <v>0</v>
@@ -10679,7 +10698,7 @@
         <v>0.94519999999999993</v>
       </c>
       <c r="K93" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L93" s="2" t="s">
@@ -10689,7 +10708,7 @@
         <v>3</v>
       </c>
       <c r="N93" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O93" s="2" t="s">
@@ -10698,73 +10717,70 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="16"/>
       <c r="R93" s="29" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F94" s="2">
+        <v>0</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H94" s="2"/>
+      <c r="J94" s="3">
+        <f>23.63/25</f>
+        <v>0.94519999999999993</v>
+      </c>
+      <c r="K94" s="3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M94" s="2">
+        <v>3</v>
+      </c>
+      <c r="N94" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O94" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="16"/>
+      <c r="R94" s="29" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C94" s="15"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="35"/>
-      <c r="J94" s="16"/>
-      <c r="K94" s="16"/>
-      <c r="Q94" s="16"/>
-      <c r="R94" s="35"/>
-    </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="F95" s="2">
-        <v>2</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="H95" s="2"/>
-      <c r="I95" s="37"/>
-      <c r="J95" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="K95" s="3">
-        <f>J95*F95</f>
-        <v>1.36</v>
-      </c>
-      <c r="L95" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M95" s="2">
-        <v>2</v>
-      </c>
-      <c r="N95" s="2">
-        <f t="shared" si="10"/>
-        <v>4</v>
-      </c>
-      <c r="O95" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="P95" s="2"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="35"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16"/>
       <c r="Q95" s="16"/>
-      <c r="R95" s="29" t="s">
-        <v>317</v>
-      </c>
-      <c r="S95" s="16"/>
-      <c r="T95" s="16"/>
-      <c r="V95" s="35"/>
+      <c r="R95" s="35"/>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
@@ -10774,17 +10790,16 @@
         <v>394</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>315</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F96" s="2">
-        <f>F95*14</f>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>360</v>
@@ -10792,21 +10807,21 @@
       <c r="H96" s="2"/>
       <c r="I96" s="37"/>
       <c r="J96" s="3">
-        <v>0.1</v>
+        <v>0.68</v>
       </c>
       <c r="K96" s="3">
         <f>J96*F96</f>
-        <v>2.8000000000000003</v>
+        <v>1.36</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M96" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N96" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>4</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>197</v>
@@ -10814,7 +10829,7 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="16"/>
       <c r="R96" s="29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="S96" s="16"/>
       <c r="T96" s="16"/>
@@ -10828,16 +10843,17 @@
         <v>394</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>315</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F97" s="2">
-        <v>2</v>
+        <f>F96*14</f>
+        <v>28</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>360</v>
@@ -10845,21 +10861,21 @@
       <c r="H97" s="2"/>
       <c r="I97" s="37"/>
       <c r="J97" s="3">
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
       <c r="K97" s="3">
         <f>J97*F97</f>
-        <v>1.5</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M97" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N97" s="2">
-        <f t="shared" si="10"/>
-        <v>4</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="O97" s="2" t="s">
         <v>197</v>
@@ -10867,7 +10883,7 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="16"/>
       <c r="R97" s="29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="S97" s="16"/>
       <c r="T97" s="16"/>
@@ -10881,17 +10897,16 @@
         <v>394</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>315</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F98" s="2">
-        <f>F97*14</f>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>360</v>
@@ -10899,21 +10914,21 @@
       <c r="H98" s="2"/>
       <c r="I98" s="37"/>
       <c r="J98" s="3">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="K98" s="3">
         <f>J98*F98</f>
-        <v>2.8000000000000003</v>
+        <v>1.5</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M98" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N98" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>4</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>197</v>
@@ -10921,7 +10936,7 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="16"/>
       <c r="R98" s="29" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="S98" s="16"/>
       <c r="T98" s="16"/>
@@ -10935,40 +10950,39 @@
         <v>394</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>384</v>
+        <v>315</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>385</v>
+        <v>325</v>
       </c>
       <c r="F99" s="2">
-        <f>2*4*6+2*2*2+2*4*1</f>
-        <v>64</v>
+        <f>F98*14</f>
+        <v>28</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="37"/>
       <c r="J99" s="3">
-        <f>19/(6*25)</f>
-        <v>0.12666666666666668</v>
+        <v>0.1</v>
       </c>
       <c r="K99" s="3">
         <f>J99*F99</f>
-        <v>8.1066666666666674</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M99" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N99" s="2">
-        <f t="shared" si="10"/>
-        <v>64</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>197</v>
@@ -10976,46 +10990,101 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="16"/>
       <c r="R99" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="S99" s="16"/>
+      <c r="T99" s="16"/>
+      <c r="V99" s="35"/>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F100" s="2">
+        <f>2*4*6+2*2*2+2*4*1</f>
+        <v>64</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H100" s="2"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="3">
+        <f>19/(6*25)</f>
+        <v>0.12666666666666668</v>
+      </c>
+      <c r="K100" s="3">
+        <f>J100*F100</f>
+        <v>8.1066666666666674</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M100" s="2">
+        <v>1</v>
+      </c>
+      <c r="N100" s="2">
+        <f t="shared" si="12"/>
+        <v>64</v>
+      </c>
+      <c r="O100" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="P100" s="2"/>
+      <c r="Q100" s="16"/>
+      <c r="R100" s="29" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="R100"/>
-    </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K101" s="5" t="s">
+      <c r="R101"/>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K102" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="N101" s="5" t="s">
+      <c r="N102" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K102" s="22">
-        <f>SUM(K1:K101)</f>
-        <v>4544.1854000000003</v>
-      </c>
-      <c r="N102" s="23">
-        <f>SUM(N1:N101)</f>
-        <v>2216.4</v>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K103" s="22">
+        <f>SUM(K1:K102)</f>
+        <v>4522.1854000000003</v>
+      </c>
+      <c r="N103" s="23">
+        <f>SUM(N1:N102)</f>
+        <v>2057</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R31" r:id="rId1"/>
     <hyperlink ref="R23" r:id="rId2"/>
-    <hyperlink ref="R60" r:id="rId3"/>
-    <hyperlink ref="R85" r:id="rId4"/>
-    <hyperlink ref="R95" r:id="rId5"/>
-    <hyperlink ref="R96" r:id="rId6"/>
-    <hyperlink ref="R97" r:id="rId7"/>
-    <hyperlink ref="R98" r:id="rId8"/>
-    <hyperlink ref="R87" r:id="rId9"/>
-    <hyperlink ref="R99" r:id="rId10"/>
-    <hyperlink ref="R92" r:id="rId11"/>
-    <hyperlink ref="R93" r:id="rId12"/>
-    <hyperlink ref="R45" r:id="rId13"/>
-    <hyperlink ref="R46" r:id="rId14"/>
+    <hyperlink ref="R61" r:id="rId3"/>
+    <hyperlink ref="R86" r:id="rId4"/>
+    <hyperlink ref="R96" r:id="rId5"/>
+    <hyperlink ref="R97" r:id="rId6"/>
+    <hyperlink ref="R98" r:id="rId7"/>
+    <hyperlink ref="R99" r:id="rId8"/>
+    <hyperlink ref="R88" r:id="rId9"/>
+    <hyperlink ref="R100" r:id="rId10"/>
+    <hyperlink ref="R93" r:id="rId11"/>
+    <hyperlink ref="R94" r:id="rId12"/>
+    <hyperlink ref="R46" r:id="rId13"/>
+    <hyperlink ref="R47" r:id="rId14"/>
     <hyperlink ref="R14" r:id="rId15"/>
     <hyperlink ref="R13" r:id="rId16"/>
     <hyperlink ref="R25" r:id="rId17"/>
@@ -11024,20 +11093,20 @@
     <hyperlink ref="R26" r:id="rId20"/>
     <hyperlink ref="R21" r:id="rId21"/>
     <hyperlink ref="R29" r:id="rId22"/>
-    <hyperlink ref="R51" r:id="rId23"/>
+    <hyperlink ref="R52" r:id="rId23"/>
     <hyperlink ref="R36" r:id="rId24"/>
-    <hyperlink ref="R37" r:id="rId25"/>
-    <hyperlink ref="R38" r:id="rId26"/>
+    <hyperlink ref="R38" r:id="rId25"/>
+    <hyperlink ref="R39" r:id="rId26"/>
     <hyperlink ref="R33" r:id="rId27"/>
     <hyperlink ref="R34" r:id="rId28"/>
-    <hyperlink ref="R52" r:id="rId29"/>
-    <hyperlink ref="R55" r:id="rId30"/>
-    <hyperlink ref="R54" r:id="rId31"/>
-    <hyperlink ref="R57" r:id="rId32"/>
-    <hyperlink ref="R49" r:id="rId33"/>
-    <hyperlink ref="R41" r:id="rId34"/>
-    <hyperlink ref="R43" r:id="rId35"/>
-    <hyperlink ref="R47" r:id="rId36"/>
+    <hyperlink ref="R53" r:id="rId29"/>
+    <hyperlink ref="R56" r:id="rId30"/>
+    <hyperlink ref="R55" r:id="rId31"/>
+    <hyperlink ref="R58" r:id="rId32"/>
+    <hyperlink ref="R50" r:id="rId33"/>
+    <hyperlink ref="R42" r:id="rId34"/>
+    <hyperlink ref="R44" r:id="rId35"/>
+    <hyperlink ref="R48" r:id="rId36"/>
     <hyperlink ref="R30" r:id="rId37"/>
     <hyperlink ref="R22" r:id="rId38"/>
     <hyperlink ref="R28" r:id="rId39"/>
@@ -11045,21 +11114,22 @@
     <hyperlink ref="R27" r:id="rId41"/>
     <hyperlink ref="R19" r:id="rId42"/>
     <hyperlink ref="R11" r:id="rId43"/>
-    <hyperlink ref="R61" r:id="rId44"/>
-    <hyperlink ref="R70" r:id="rId45"/>
+    <hyperlink ref="R62" r:id="rId44"/>
+    <hyperlink ref="R71" r:id="rId45"/>
     <hyperlink ref="R15" r:id="rId46"/>
-    <hyperlink ref="R83" r:id="rId47"/>
-    <hyperlink ref="R84" r:id="rId48"/>
-    <hyperlink ref="R80" r:id="rId49"/>
-    <hyperlink ref="R81" r:id="rId50"/>
-    <hyperlink ref="R82" r:id="rId51"/>
-    <hyperlink ref="R79" r:id="rId52"/>
-    <hyperlink ref="R72" r:id="rId53"/>
-    <hyperlink ref="R73" r:id="rId54"/>
-    <hyperlink ref="R74" r:id="rId55"/>
+    <hyperlink ref="R84" r:id="rId47"/>
+    <hyperlink ref="R85" r:id="rId48"/>
+    <hyperlink ref="R81" r:id="rId49"/>
+    <hyperlink ref="R82" r:id="rId50"/>
+    <hyperlink ref="R83" r:id="rId51"/>
+    <hyperlink ref="R80" r:id="rId52"/>
+    <hyperlink ref="R73" r:id="rId53"/>
+    <hyperlink ref="R74" r:id="rId54"/>
+    <hyperlink ref="R75" r:id="rId55"/>
+    <hyperlink ref="R37" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 
@@ -12353,7 +12423,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>